<commit_message>
Preprocessing for selecting best K in Kmeans, merging some chunks of data together, solving some other minors issues
</commit_message>
<xml_diff>
--- a/dq/score/assertions_score_weighting_definition.xlsx
+++ b/dq/score/assertions_score_weighting_definition.xlsx
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>